<commit_message>
using mrg v1.00.01 and tweaking fig
</commit_message>
<xml_diff>
--- a/data/benchmark_evaluation/smvar HG002 MRG v0.03.00 evaluation.xlsx
+++ b/data/benchmark_evaluation/smvar HG002 MRG v0.03.00 evaluation.xlsx
@@ -9800,7 +9800,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>

</xml_diff>